<commit_message>
replace row.names with name column
</commit_message>
<xml_diff>
--- a/inst/extdata/demo_template.xlsx
+++ b/inst/extdata/demo_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/chilliwack-exploit-upload/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandalgarno/Code/chktemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A786D5-DCB6-2841-8FB3-BB11CFB697AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE85735-BCA0-6946-8E8D-1BBE464508DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27720" windowHeight="17040" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27720" windowHeight="17040" activeTab="2" xr2:uid="{D2F727D3-E3E6-DE42-943C-87973B24BE7C}"/>
   </bookViews>
   <sheets>
     <sheet name="outing" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -290,15 +290,6 @@
   </si>
   <si>
     <t>lure type used in capture</t>
-  </si>
-  <si>
-    <t>recapture</t>
-  </si>
-  <si>
-    <t>capture</t>
-  </si>
-  <si>
-    <t>outing</t>
   </si>
   <si>
     <t>chk</t>
@@ -738,9 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D07577A-358A-F34F-9161-33686BFF2FB9}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -763,7 +752,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
@@ -892,63 +881,63 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>90</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" t="s">
         <v>91</v>
-      </c>
-      <c r="F4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" t="s">
-        <v>102</v>
-      </c>
-      <c r="M4" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" t="s">
-        <v>101</v>
-      </c>
-      <c r="O4" t="s">
-        <v>101</v>
-      </c>
-      <c r="P4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>106</v>
-      </c>
-      <c r="R4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1067,9 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B9C42-9339-A047-901C-9A85D8DE94F1}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1094,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
@@ -1235,63 +1222,63 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" t="s">
         <v>95</v>
       </c>
-      <c r="J4" t="s">
-        <v>103</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="P4" t="s">
         <v>96</v>
       </c>
-      <c r="L4" t="s">
-        <v>97</v>
-      </c>
-      <c r="M4" t="s">
-        <v>113</v>
-      </c>
-      <c r="N4" t="s">
-        <v>113</v>
-      </c>
-      <c r="O4" t="s">
-        <v>98</v>
-      </c>
-      <c r="P4" t="s">
-        <v>99</v>
-      </c>
       <c r="Q4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="R4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1410,9 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5014DBCF-9011-9A47-9D03-DDE81D462BF0}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1431,7 +1416,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1518,42 +1503,42 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" t="s">
         <v>91</v>
-      </c>
-      <c r="E4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>

</xml_diff>